<commit_message>
mise a jour ReadMe
</commit_message>
<xml_diff>
--- a/kicad/shield_gas_sensor/shield_gas_sensor.xlsx
+++ b/kicad/shield_gas_sensor/shield_gas_sensor.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Documents\_FRANCOIS\_INSA\MOSH\2021_2022_Saillard_Grau\kicad\shield_gas_sensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F24A41E8-4E2A-4DBC-A947-6667156AECCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8E65A3-9CB6-4B47-A88B-FF80845F7CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shield_gas_sensor" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="84">
   <si>
     <t>Source:</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Vendor</t>
   </si>
   <si>
     <t>100n</t>
@@ -280,8 +277,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,8 +413,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -597,8 +603,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -713,6 +725,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -758,14 +822,35 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1121,570 +1206,553 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.08984375" customWidth="1"/>
-    <col min="2" max="2" width="6.54296875" customWidth="1"/>
-    <col min="4" max="4" width="25.6328125" customWidth="1"/>
-    <col min="5" max="5" width="37.90625" customWidth="1"/>
-    <col min="9" max="9" width="30.81640625" customWidth="1"/>
-    <col min="10" max="10" width="26.90625" customWidth="1"/>
+    <col min="1" max="1" width="20.08984375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6.54296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" style="2"/>
+    <col min="4" max="4" width="25.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="37.90625" style="2" customWidth="1"/>
+    <col min="6" max="8" width="10.90625" style="2"/>
+    <col min="9" max="9" width="26.90625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="10.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>44563.779236111113</v>
       </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B11" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I11" t="s">
+      <c r="G11" s="11"/>
+      <c r="H11" s="12"/>
+    </row>
+    <row r="12" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="6">
+        <v>3</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="D12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="6">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="6">
+        <v>1</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B12">
+      <c r="B17" s="6">
+        <v>2</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="6">
+        <v>2</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="6">
+        <v>1</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="6">
+        <v>1</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="6">
+        <v>1</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="6">
         <v>3</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13">
+      <c r="C23" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="6">
+        <v>2</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="6">
+        <v>2</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="6">
         <v>1</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-    </row>
-    <row r="14" spans="1:12" ht="58" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14">
+      <c r="C26" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="6">
         <v>1</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-    </row>
-    <row r="15" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15">
+      <c r="C27" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="6">
         <v>1</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-    </row>
-    <row r="17" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-    </row>
-    <row r="21" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-    </row>
-    <row r="22" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-    </row>
-    <row r="23" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B23">
-        <v>3</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-    </row>
-    <row r="24" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B24">
-        <v>2</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-    </row>
-    <row r="26" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-    </row>
-    <row r="27" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
+      <c r="C28" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F11:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>